<commit_message>
Solved problem with the MySQL column names, they weren't find in the right order any more
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1598463917" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1598463917" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1598463917" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1598463917"/>
+      <pm:revision xmlns:pm="smNativeData" day="1613554366" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1613554366" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1613554366" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1613554366"/>
     </ext>
   </extLst>
 </workbook>
@@ -1280,8 +1280,8 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="20" formatCode="h:mm"/>
     <numFmt numFmtId="11" formatCode="0.00E+00"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YYYY;@"/>
+    <numFmt numFmtId="14" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1291,7 +1291,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598463917" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613554366" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1306,7 +1306,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598463917" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613554366" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1322,7 +1322,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598463917" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613554366" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1337,7 +1337,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598463917" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1613554366" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1398,7 +1398,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1598463917" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1613554366" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1420,7 +1420,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917"/>
+          <pm:border xmlns:pm="smNativeData" id="1613554366"/>
         </ext>
       </extLst>
     </border>
@@ -1439,7 +1439,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1460,7 +1460,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1482,7 +1482,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1503,7 +1503,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1524,7 +1524,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1545,7 +1545,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1567,7 +1567,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1589,7 +1589,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1612,7 +1612,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1634,7 +1634,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1657,7 +1657,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1679,7 +1679,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1701,7 +1701,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917">
+          <pm:border xmlns:pm="smNativeData" id="1613554366">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1723,7 +1723,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598463917"/>
+          <pm:border xmlns:pm="smNativeData" id="1613554366"/>
         </ext>
       </extLst>
     </border>
@@ -1791,20 +1791,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1812,10 +1812,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1598463917" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1613554366" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1598463917" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1613554366" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -2081,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N624"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A561" workbookViewId="0">
-      <selection activeCell="C584" sqref="C584"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A465" workbookViewId="0">
+      <selection activeCell="L474" sqref="L474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
@@ -2097,14 +2097,14 @@
     <col min="9" max="9" width="23.000000" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1598463917" min="9" max="9" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613554366" min="9" max="9" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
     <col min="10" max="10" width="15.660714" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1598463917" min="10" max="10" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613554366" min="10" max="10" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
@@ -2112,14 +2112,14 @@
     <col min="13" max="13" width="13.107143" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1598463917" min="13" max="13" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613554366" min="13" max="13" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
     <col min="14" max="14" width="14.000000" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1598463917" min="14" max="14" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1613554366" min="14" max="14" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
@@ -11901,7 +11901,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="589" spans="1:4">
+    <row r="589" spans="1:5">
       <c r="A589" t="n">
         <v>588</v>
       </c>
@@ -11910,6 +11910,9 @@
       </c>
       <c r="D589" s="19" t="s">
         <v>371</v>
+      </c>
+      <c r="E589" s="33" t="n">
+        <v>44069</v>
       </c>
     </row>
     <row r="590" spans="1:1">
@@ -12091,7 +12094,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1598463917" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613554366" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -12100,14 +12103,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1598463917" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1598463917" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613554366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613554366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1598463917" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613554366" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -12129,7 +12132,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1598463917" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613554366" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -12138,14 +12141,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1598463917" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1598463917" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613554366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613554366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1598463917" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613554366" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -12167,7 +12170,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1598463917" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1613554366" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -12176,14 +12179,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1598463917" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1598463917" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1613554366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1613554366" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1598463917" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1613554366" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>